<commit_message>
Updated BOM.xlsx and added most of the 3D models
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -52,10 +52,13 @@
     <t>Preferably the HexTech-designated power source, but can be anything</t>
   </si>
   <si>
-    <t>Blades (More Specific)</t>
+    <t>WORKPRO Utility Knife Blades</t>
   </si>
   <si>
-    <t>Usually Come in Packs of many</t>
+    <t>1 pack</t>
+  </si>
+  <si>
+    <t>This is the specific blade that fits into the housing</t>
   </si>
   <si>
     <t>Extruder</t>
@@ -598,13 +601,15 @@
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="4">
-        <v>2.0</v>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="9">
+        <v>10.0</v>
+      </c>
       <c r="D6" s="5"/>
       <c r="E6" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -630,7 +635,7 @@
     </row>
     <row r="7" ht="19.5" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="7">
         <v>1.0</v>
@@ -640,7 +645,7 @@
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
@@ -666,7 +671,7 @@
     </row>
     <row r="8" ht="36.75" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="4">
         <v>2.0</v>
@@ -676,7 +681,7 @@
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
@@ -702,17 +707,17 @@
     </row>
     <row r="9" ht="19.5" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" s="7">
         <v>2.0</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
@@ -738,7 +743,7 @@
     </row>
     <row r="10" ht="19.5" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" s="4">
         <v>7.0</v>
@@ -748,7 +753,7 @@
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
@@ -28494,8 +28499,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="C8"/>
+    <hyperlink r:id="rId1" ref="C6"/>
+    <hyperlink r:id="rId2" ref="C8"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>